<commit_message>
Modifico el registro masivo de usuarios
</commit_message>
<xml_diff>
--- a/public/excel/FORMATO EXCEL.xlsx
+++ b/public/excel/FORMATO EXCEL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alend\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Instr Diego Calderon\Formatrack\Backendnestjs\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86789CD3-E9F3-44AE-AF6C-C0972D5DA4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9DA1A9-7ADA-484B-9C67-80ABDE8731F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C2BD731E-F99D-41EC-8951-20E87AAE127A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C2BD731E-F99D-41EC-8951-20E87AAE127A}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>documento</t>
   </si>
@@ -60,19 +60,13 @@
   </si>
   <si>
     <t>cargo</t>
-  </si>
-  <si>
-    <t>perfil</t>
-  </si>
-  <si>
-    <t>fkrol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,12 +109,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -465,12 +465,12 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -495,14 +495,10 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -515,7 +511,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -528,7 +524,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -541,7 +537,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -554,7 +550,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -563,11 +559,11 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="I6" s="3"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -580,7 +576,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -593,7 +589,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -606,7 +602,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -619,7 +615,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
Modifico el excel por defecto y dejo estado en true
</commit_message>
<xml_diff>
--- a/public/excel/FORMATO EXCEL.xlsx
+++ b/public/excel/FORMATO EXCEL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Instr Diego Calderon\Formatrack\Backendnestjs\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9DA1A9-7ADA-484B-9C67-80ABDE8731F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831AA3CD-7538-4AE9-8F73-D0819D936A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C2BD731E-F99D-41EC-8951-20E87AAE127A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>documento</t>
   </si>
@@ -45,21 +45,6 @@
   </si>
   <si>
     <t>apellido</t>
-  </si>
-  <si>
-    <t>edad</t>
-  </si>
-  <si>
-    <t>telefono</t>
-  </si>
-  <si>
-    <t>correo</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>cargo</t>
   </si>
 </sst>
 </file>
@@ -117,8 +102,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -465,7 +450,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,23 +465,13 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -559,7 +534,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>

</xml_diff>